<commit_message>
done animations and update map
</commit_message>
<xml_diff>
--- a/resources/maps/map1.xlsx
+++ b/resources/maps/map1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,877 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="138">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -863,12 +1733,12 @@
   <dimension ref="A1:BL48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BQ20" sqref="BQ20"/>
+      <selection activeCell="BS24" sqref="BS24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="64" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="64" width="1.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" x14ac:dyDescent="0.35">
@@ -1288,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1300,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -1354,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="AF3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG3">
         <v>0</v>
@@ -1387,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="AQ3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR3">
         <v>0</v>
@@ -1402,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="AV3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW3">
         <v>0</v>
@@ -1494,7 +2364,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -1548,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="AF4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG4">
         <v>0</v>
@@ -1581,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="AQ4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR4">
         <v>0</v>
@@ -1688,7 +2558,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -1742,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="AF5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG5">
         <v>0</v>
@@ -1775,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="AQ5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR5">
         <v>0</v>
@@ -1882,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -1936,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="AF6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG6">
         <v>0</v>
@@ -1969,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="AQ6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR6">
         <v>0</v>
@@ -2076,7 +2946,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -2151,7 +3021,7 @@
         <v>0</v>
       </c>
       <c r="AM7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AN7">
         <v>0</v>
@@ -2163,7 +3033,7 @@
         <v>0</v>
       </c>
       <c r="AQ7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR7">
         <v>0</v>
@@ -2270,7 +3140,7 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -2357,7 +3227,7 @@
         <v>0</v>
       </c>
       <c r="AQ8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR8">
         <v>0</v>
@@ -2464,7 +3334,7 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -2551,7 +3421,7 @@
         <v>0</v>
       </c>
       <c r="AQ9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR9">
         <v>0</v>
@@ -2658,7 +3528,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -2745,7 +3615,7 @@
         <v>0</v>
       </c>
       <c r="AQ10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR10">
         <v>0</v>
@@ -2852,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -2939,7 +3809,7 @@
         <v>0</v>
       </c>
       <c r="AQ11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR11">
         <v>0</v>
@@ -3010,190 +3880,190 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF12">
         <v>3</v>
       </c>
       <c r="AG12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AT12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AU12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AV12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AW12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AX12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BB12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BD12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BE12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BF12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BG12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BH12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BI12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BJ12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BK12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BL12">
         <v>9</v>
@@ -4458,7 +5328,7 @@
         <v>0</v>
       </c>
       <c r="AF19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG19">
         <v>0</v>
@@ -4562,61 +5432,61 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U20">
         <v>2</v>
@@ -4688,64 +5558,64 @@
         <v>2</v>
       </c>
       <c r="AR20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AV20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AX20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AY20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AZ20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BC20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BD20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BE20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BF20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BG20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BH20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BI20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BJ20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BK20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BL20">
         <v>9</v>
@@ -4846,7 +5716,7 @@
         <v>0</v>
       </c>
       <c r="AF21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG21">
         <v>0</v>
@@ -5920,190 +6790,190 @@
         <v>9</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF27">
         <v>3</v>
       </c>
       <c r="AG27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AT27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AU27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AV27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AW27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AX27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BB27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BD27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BE27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BF27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BG27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BH27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BI27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BJ27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BK27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BL27">
         <v>9</v>
@@ -6165,7 +7035,7 @@
         <v>0</v>
       </c>
       <c r="S28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T28">
         <v>0</v>
@@ -6204,7 +7074,7 @@
         <v>0</v>
       </c>
       <c r="AF28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG28">
         <v>0</v>
@@ -6234,7 +7104,7 @@
         <v>0</v>
       </c>
       <c r="AP28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ28">
         <v>0</v>
@@ -6359,7 +7229,7 @@
         <v>0</v>
       </c>
       <c r="S29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T29">
         <v>0</v>
@@ -6398,7 +7268,7 @@
         <v>0</v>
       </c>
       <c r="AF29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG29">
         <v>0</v>
@@ -6428,7 +7298,7 @@
         <v>0</v>
       </c>
       <c r="AP29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ29">
         <v>0</v>
@@ -6553,7 +7423,7 @@
         <v>0</v>
       </c>
       <c r="S30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T30">
         <v>0</v>
@@ -6592,7 +7462,7 @@
         <v>0</v>
       </c>
       <c r="AF30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG30">
         <v>0</v>
@@ -6622,7 +7492,7 @@
         <v>0</v>
       </c>
       <c r="AP30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ30">
         <v>0</v>
@@ -6747,7 +7617,7 @@
         <v>0</v>
       </c>
       <c r="S31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T31">
         <v>0</v>
@@ -6786,7 +7656,7 @@
         <v>0</v>
       </c>
       <c r="AF31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG31">
         <v>0</v>
@@ -6816,7 +7686,7 @@
         <v>0</v>
       </c>
       <c r="AP31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ31">
         <v>0</v>
@@ -6941,7 +7811,7 @@
         <v>0</v>
       </c>
       <c r="S32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T32">
         <v>0</v>
@@ -6980,7 +7850,7 @@
         <v>0</v>
       </c>
       <c r="AF32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG32">
         <v>0</v>
@@ -7010,7 +7880,7 @@
         <v>0</v>
       </c>
       <c r="AP32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ32">
         <v>0</v>
@@ -7135,7 +8005,7 @@
         <v>0</v>
       </c>
       <c r="S33">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="T33">
         <v>0</v>
@@ -7174,7 +8044,7 @@
         <v>0</v>
       </c>
       <c r="AF33">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG33">
         <v>0</v>
@@ -7204,7 +8074,7 @@
         <v>0</v>
       </c>
       <c r="AP33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ33">
         <v>0</v>
@@ -7317,7 +8187,7 @@
         <v>0</v>
       </c>
       <c r="O34">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P34">
         <v>0</v>
@@ -7329,7 +8199,7 @@
         <v>0</v>
       </c>
       <c r="S34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T34">
         <v>0</v>
@@ -7368,7 +8238,7 @@
         <v>0</v>
       </c>
       <c r="AF34">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG34">
         <v>0</v>
@@ -7398,7 +8268,7 @@
         <v>0</v>
       </c>
       <c r="AP34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ34">
         <v>5</v>
@@ -7523,7 +8393,7 @@
         <v>0</v>
       </c>
       <c r="S35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T35">
         <v>0</v>
@@ -7562,7 +8432,7 @@
         <v>6</v>
       </c>
       <c r="AF35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG35">
         <v>0</v>
@@ -7592,7 +8462,7 @@
         <v>0</v>
       </c>
       <c r="AP35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ35">
         <v>0</v>
@@ -7616,46 +8486,46 @@
         <v>0</v>
       </c>
       <c r="AX35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BB35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BD35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BE35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BF35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BG35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BH35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BI35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BJ35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BK35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BL35">
         <v>9</v>
@@ -7717,7 +8587,7 @@
         <v>0</v>
       </c>
       <c r="S36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T36">
         <v>0</v>
@@ -7756,7 +8626,7 @@
         <v>0</v>
       </c>
       <c r="AF36">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG36">
         <v>0</v>
@@ -7786,7 +8656,7 @@
         <v>0</v>
       </c>
       <c r="AP36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ36">
         <v>0</v>
@@ -7810,7 +8680,7 @@
         <v>0</v>
       </c>
       <c r="AX36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY36">
         <v>0</v>
@@ -7911,7 +8781,7 @@
         <v>0</v>
       </c>
       <c r="S37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T37">
         <v>0</v>
@@ -7950,7 +8820,7 @@
         <v>0</v>
       </c>
       <c r="AF37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG37">
         <v>0</v>
@@ -7980,7 +8850,7 @@
         <v>0</v>
       </c>
       <c r="AP37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ37">
         <v>0</v>
@@ -8004,7 +8874,7 @@
         <v>0</v>
       </c>
       <c r="AX37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY37">
         <v>0</v>
@@ -8105,7 +8975,7 @@
         <v>0</v>
       </c>
       <c r="S38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T38">
         <v>0</v>
@@ -8144,7 +9014,7 @@
         <v>0</v>
       </c>
       <c r="AF38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG38">
         <v>0</v>
@@ -8174,7 +9044,7 @@
         <v>0</v>
       </c>
       <c r="AP38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ38">
         <v>0</v>
@@ -8198,7 +9068,7 @@
         <v>0</v>
       </c>
       <c r="AX38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY38">
         <v>0</v>
@@ -8299,7 +9169,7 @@
         <v>0</v>
       </c>
       <c r="S39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T39">
         <v>0</v>
@@ -8338,7 +9208,7 @@
         <v>0</v>
       </c>
       <c r="AF39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG39">
         <v>0</v>
@@ -8368,7 +9238,7 @@
         <v>0</v>
       </c>
       <c r="AP39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ39">
         <v>0</v>
@@ -8392,7 +9262,7 @@
         <v>0</v>
       </c>
       <c r="AX39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY39">
         <v>0</v>
@@ -8493,7 +9363,7 @@
         <v>0</v>
       </c>
       <c r="S40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T40">
         <v>0</v>
@@ -8532,7 +9402,7 @@
         <v>0</v>
       </c>
       <c r="AF40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG40">
         <v>0</v>
@@ -8562,7 +9432,7 @@
         <v>0</v>
       </c>
       <c r="AP40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ40">
         <v>0</v>
@@ -8586,7 +9456,7 @@
         <v>0</v>
       </c>
       <c r="AX40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY40">
         <v>0</v>
@@ -8687,7 +9557,7 @@
         <v>0</v>
       </c>
       <c r="S41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T41">
         <v>0</v>
@@ -8726,7 +9596,7 @@
         <v>0</v>
       </c>
       <c r="AF41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG41">
         <v>0</v>
@@ -8756,7 +9626,7 @@
         <v>0</v>
       </c>
       <c r="AP41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ41">
         <v>0</v>
@@ -8780,7 +9650,7 @@
         <v>0</v>
       </c>
       <c r="AX41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY41">
         <v>0</v>
@@ -8881,7 +9751,7 @@
         <v>0</v>
       </c>
       <c r="S42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T42">
         <v>0</v>
@@ -8920,7 +9790,7 @@
         <v>0</v>
       </c>
       <c r="AF42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG42">
         <v>0</v>
@@ -8950,7 +9820,7 @@
         <v>0</v>
       </c>
       <c r="AP42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ42">
         <v>0</v>
@@ -8968,13 +9838,13 @@
         <v>0</v>
       </c>
       <c r="AV42">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AW42">
         <v>0</v>
       </c>
       <c r="AX42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY42">
         <v>0</v>
@@ -9075,7 +9945,7 @@
         <v>0</v>
       </c>
       <c r="S43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T43">
         <v>0</v>
@@ -9084,7 +9954,7 @@
         <v>0</v>
       </c>
       <c r="V43">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="W43">
         <v>0</v>
@@ -9114,7 +9984,7 @@
         <v>0</v>
       </c>
       <c r="AF43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG43">
         <v>0</v>
@@ -9144,7 +10014,7 @@
         <v>0</v>
       </c>
       <c r="AP43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ43">
         <v>0</v>
@@ -9168,7 +10038,7 @@
         <v>0</v>
       </c>
       <c r="AX43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY43">
         <v>0</v>
@@ -9269,7 +10139,7 @@
         <v>0</v>
       </c>
       <c r="S44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T44">
         <v>0</v>
@@ -9308,7 +10178,7 @@
         <v>0</v>
       </c>
       <c r="AF44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG44">
         <v>0</v>
@@ -9338,7 +10208,7 @@
         <v>0</v>
       </c>
       <c r="AP44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ44">
         <v>0</v>
@@ -9362,7 +10232,7 @@
         <v>0</v>
       </c>
       <c r="AX44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY44">
         <v>0</v>
@@ -9463,7 +10333,7 @@
         <v>0</v>
       </c>
       <c r="S45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T45">
         <v>0</v>
@@ -9502,7 +10372,7 @@
         <v>0</v>
       </c>
       <c r="AF45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG45">
         <v>0</v>
@@ -9532,7 +10402,7 @@
         <v>0</v>
       </c>
       <c r="AP45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ45">
         <v>0</v>
@@ -9556,7 +10426,7 @@
         <v>0</v>
       </c>
       <c r="AX45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY45">
         <v>0</v>
@@ -9657,7 +10527,7 @@
         <v>0</v>
       </c>
       <c r="S46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T46">
         <v>0</v>
@@ -9690,13 +10560,13 @@
         <v>0</v>
       </c>
       <c r="AD46">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE46">
         <v>0</v>
       </c>
       <c r="AF46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG46">
         <v>0</v>
@@ -9726,7 +10596,7 @@
         <v>0</v>
       </c>
       <c r="AP46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ46">
         <v>0</v>
@@ -9750,7 +10620,7 @@
         <v>0</v>
       </c>
       <c r="AX46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY46">
         <v>0</v>
@@ -9851,7 +10721,7 @@
         <v>0</v>
       </c>
       <c r="S47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T47">
         <v>0</v>
@@ -9890,7 +10760,7 @@
         <v>0</v>
       </c>
       <c r="AF47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG47">
         <v>0</v>
@@ -9920,7 +10790,7 @@
         <v>0</v>
       </c>
       <c r="AP47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ47">
         <v>0</v>
@@ -9944,7 +10814,7 @@
         <v>0</v>
       </c>
       <c r="AX47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY47">
         <v>0</v>
@@ -10185,32 +11055,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AM9">
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR14">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="4" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10224,7 +11094,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10236,7 +11106,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update background images, organize sounds, implement and handle more buttons and functions
</commit_message>
<xml_diff>
--- a/resources/maps/map1.xlsx
+++ b/resources/maps/map1.xlsx
@@ -7,9 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="map1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -52,1307 +50,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="138">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1732,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BS24" sqref="BS24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AW7" sqref="AW7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1976,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -2030,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG2">
         <v>0</v>
@@ -2090,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="AZ2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA2">
         <v>0</v>
@@ -2257,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="AQ3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR3">
         <v>0</v>
@@ -2284,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="AZ3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA3">
         <v>0</v>
@@ -2352,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -2451,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="AQ4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR4">
         <v>0</v>
@@ -2466,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="AV4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW4">
         <v>0</v>
@@ -2478,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="AZ4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA4">
         <v>0</v>
@@ -2546,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -2579,11 +1277,11 @@
         <v>0</v>
       </c>
       <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
         <v>4</v>
       </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
       <c r="W5">
         <v>0</v>
       </c>
@@ -2642,10 +1340,10 @@
         <v>0</v>
       </c>
       <c r="AP5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AQ5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR5">
         <v>0</v>
@@ -2660,7 +1358,7 @@
         <v>0</v>
       </c>
       <c r="AV5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW5">
         <v>0</v>
@@ -2672,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="AZ5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA5">
         <v>0</v>
@@ -2740,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -2752,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -2839,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="AQ6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR6">
         <v>0</v>
@@ -2854,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="AV6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW6">
         <v>0</v>
@@ -2866,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="AZ6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA6">
         <v>0</v>
@@ -2934,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -2946,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -3000,7 +1698,7 @@
         <v>0</v>
       </c>
       <c r="AF7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG7">
         <v>0</v>
@@ -3021,7 +1719,7 @@
         <v>0</v>
       </c>
       <c r="AM7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AN7">
         <v>0</v>
@@ -3033,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="AQ7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR7">
         <v>0</v>
@@ -3048,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="AV7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW7">
         <v>0</v>
@@ -3060,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="AZ7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA7">
         <v>0</v>
@@ -3113,22 +1811,22 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -3140,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -3194,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="AF8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG8">
         <v>0</v>
@@ -3227,7 +1925,7 @@
         <v>0</v>
       </c>
       <c r="AQ8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR8">
         <v>0</v>
@@ -3242,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="AV8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW8">
         <v>0</v>
@@ -3254,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="AZ8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA8">
         <v>0</v>
@@ -3334,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -3388,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="AF9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG9">
         <v>0</v>
@@ -3421,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="AQ9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR9">
         <v>0</v>
@@ -3436,37 +2134,37 @@
         <v>0</v>
       </c>
       <c r="AV9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AX9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AY9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AZ9">
         <v>3</v>
       </c>
       <c r="BA9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BB9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BC9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BD9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BE9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BF9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BG9">
         <v>0</v>
@@ -3492,43 +2190,43 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -3582,7 +2280,7 @@
         <v>0</v>
       </c>
       <c r="AF10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG10">
         <v>0</v>
@@ -3615,7 +2313,7 @@
         <v>0</v>
       </c>
       <c r="AQ10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR10">
         <v>0</v>
@@ -3642,40 +2340,40 @@
         <v>0</v>
       </c>
       <c r="AZ10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BC10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BD10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BE10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BF10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BG10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BH10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BI10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BJ10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BK10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BL10">
         <v>9</v>
@@ -3722,7 +2420,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -3794,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="AL11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM11">
         <v>0</v>
@@ -3809,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="AQ11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR11">
         <v>0</v>
@@ -3880,190 +2578,190 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Y12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AB12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AD12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF12">
         <v>3</v>
       </c>
       <c r="AG12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AH12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AI12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AK12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AL12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AM12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AN12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AO12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AP12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AQ12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AR12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AS12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AT12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AU12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AV12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AX12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BA12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BB12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BC12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BD12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BE12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="BG12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BH12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BI12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BJ12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BK12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BL12">
         <v>9</v>
@@ -4200,7 +2898,7 @@
         <v>0</v>
       </c>
       <c r="AR13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AS13">
         <v>0</v>
@@ -4274,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -4519,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="U15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -4656,190 +3354,190 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF16">
         <v>3</v>
       </c>
       <c r="AG16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AV16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AX16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AY16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AZ16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BC16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BD16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BE16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BF16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BG16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BH16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BI16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BJ16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BK16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BL16">
         <v>9</v>
@@ -5068,7 +3766,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -5328,7 +4026,7 @@
         <v>0</v>
       </c>
       <c r="AF19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG19">
         <v>0</v>
@@ -5352,7 +4050,7 @@
         <v>0</v>
       </c>
       <c r="AN19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO19">
         <v>0</v>
@@ -5432,190 +4130,190 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AI20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AP20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AU20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AV20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AX20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AY20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AZ20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BA20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BB20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BC20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BD20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BE20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BF20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BG20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BI20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BJ20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BK20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BL20">
         <v>9</v>
@@ -5716,7 +4414,7 @@
         <v>0</v>
       </c>
       <c r="AF21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG21">
         <v>0</v>
@@ -5803,7 +4501,7 @@
         <v>0</v>
       </c>
       <c r="BI21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BJ21">
         <v>0</v>
@@ -5826,7 +4524,7 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -5901,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="AC22">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD22">
         <v>0</v>
@@ -5940,7 +4638,7 @@
         <v>0</v>
       </c>
       <c r="AP22">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AQ22">
         <v>0</v>
@@ -6026,7 +4724,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -6208,190 +4906,190 @@
         <v>9</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V24">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="W24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF24">
         <v>3</v>
       </c>
       <c r="AG24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AS24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AT24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AU24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AV24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AW24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AX24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BB24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BD24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BE24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BF24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BG24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BH24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BI24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BJ24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BK24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BL24">
         <v>9</v>
@@ -6573,7 +5271,7 @@
         <v>0</v>
       </c>
       <c r="BG25">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BH25">
         <v>0</v>
@@ -6638,7 +5336,7 @@
         <v>0</v>
       </c>
       <c r="P26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -6710,7 +5408,7 @@
         <v>0</v>
       </c>
       <c r="AN26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AO26">
         <v>0</v>
@@ -6790,190 +5488,190 @@
         <v>9</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AB27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AD27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF27">
         <v>3</v>
       </c>
       <c r="AG27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AH27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AI27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AK27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AL27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AM27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AN27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AO27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AP27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AQ27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AR27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AS27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AT27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AU27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AV27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AX27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BA27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BB27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BC27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BD27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BE27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BG27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BH27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BI27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BJ27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BK27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BL27">
         <v>9</v>
@@ -7035,7 +5733,7 @@
         <v>0</v>
       </c>
       <c r="S28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T28">
         <v>0</v>
@@ -7104,7 +5802,7 @@
         <v>0</v>
       </c>
       <c r="AP28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ28">
         <v>0</v>
@@ -7137,13 +5835,13 @@
         <v>0</v>
       </c>
       <c r="BA28">
+        <v>0</v>
+      </c>
+      <c r="BB28">
+        <v>0</v>
+      </c>
+      <c r="BC28">
         <v>4</v>
-      </c>
-      <c r="BB28">
-        <v>0</v>
-      </c>
-      <c r="BC28">
-        <v>0</v>
       </c>
       <c r="BD28">
         <v>0</v>
@@ -7229,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="S29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T29">
         <v>0</v>
@@ -7298,7 +5996,7 @@
         <v>0</v>
       </c>
       <c r="AP29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ29">
         <v>0</v>
@@ -7393,17 +6091,17 @@
         <v>0</v>
       </c>
       <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
         <v>5</v>
       </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
       <c r="M30">
         <v>0</v>
       </c>
@@ -7423,7 +6121,7 @@
         <v>0</v>
       </c>
       <c r="S30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T30">
         <v>0</v>
@@ -7447,7 +6145,7 @@
         <v>0</v>
       </c>
       <c r="AA30">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AB30">
         <v>0</v>
@@ -7468,7 +6166,7 @@
         <v>0</v>
       </c>
       <c r="AH30">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AI30">
         <v>0</v>
@@ -7492,7 +6190,7 @@
         <v>0</v>
       </c>
       <c r="AP30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ30">
         <v>0</v>
@@ -7546,7 +6244,7 @@
         <v>0</v>
       </c>
       <c r="BH30">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BI30">
         <v>0</v>
@@ -7617,7 +6315,7 @@
         <v>0</v>
       </c>
       <c r="S31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T31">
         <v>0</v>
@@ -7686,7 +6384,7 @@
         <v>0</v>
       </c>
       <c r="AP31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ31">
         <v>0</v>
@@ -7760,190 +6458,190 @@
         <v>9</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S32">
         <v>2</v>
       </c>
       <c r="T32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF32">
         <v>3</v>
       </c>
       <c r="AG32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP32">
         <v>2</v>
       </c>
       <c r="AQ32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AV32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AX32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AY32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AZ32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BC32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BD32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BE32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BF32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BG32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BH32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BI32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BJ32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BK32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BL32">
         <v>9</v>
@@ -8005,7 +6703,7 @@
         <v>0</v>
       </c>
       <c r="S33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T33">
         <v>0</v>
@@ -8074,7 +6772,7 @@
         <v>0</v>
       </c>
       <c r="AP33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ33">
         <v>0</v>
@@ -8119,7 +6817,7 @@
         <v>0</v>
       </c>
       <c r="BE33">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BF33">
         <v>0</v>
@@ -8187,7 +6885,7 @@
         <v>0</v>
       </c>
       <c r="O34">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P34">
         <v>0</v>
@@ -8199,7 +6897,7 @@
         <v>0</v>
       </c>
       <c r="S34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T34">
         <v>0</v>
@@ -8268,10 +6966,10 @@
         <v>0</v>
       </c>
       <c r="AP34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ34">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AR34">
         <v>0</v>
@@ -8354,7 +7052,7 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -8393,7 +7091,7 @@
         <v>0</v>
       </c>
       <c r="S35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T35">
         <v>0</v>
@@ -8429,7 +7127,7 @@
         <v>0</v>
       </c>
       <c r="AE35">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AF35">
         <v>3</v>
@@ -8462,7 +7160,7 @@
         <v>0</v>
       </c>
       <c r="AP35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ35">
         <v>0</v>
@@ -8486,46 +7184,46 @@
         <v>0</v>
       </c>
       <c r="AX35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BA35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BB35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BC35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BD35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BE35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BG35">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="BH35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BI35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BJ35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BK35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BL35">
         <v>9</v>
@@ -8587,7 +7285,7 @@
         <v>0</v>
       </c>
       <c r="S36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T36">
         <v>0</v>
@@ -8611,7 +7309,7 @@
         <v>0</v>
       </c>
       <c r="AA36">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB36">
         <v>0</v>
@@ -8650,13 +7348,13 @@
         <v>0</v>
       </c>
       <c r="AN36">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AO36">
         <v>0</v>
       </c>
       <c r="AP36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ36">
         <v>0</v>
@@ -8680,7 +7378,7 @@
         <v>0</v>
       </c>
       <c r="AX36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY36">
         <v>0</v>
@@ -8781,7 +7479,7 @@
         <v>0</v>
       </c>
       <c r="S37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T37">
         <v>0</v>
@@ -8850,7 +7548,7 @@
         <v>0</v>
       </c>
       <c r="AP37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ37">
         <v>0</v>
@@ -8874,7 +7572,7 @@
         <v>0</v>
       </c>
       <c r="AX37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY37">
         <v>0</v>
@@ -8924,43 +7622,43 @@
         <v>9</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O38">
         <v>0</v>
@@ -8975,7 +7673,7 @@
         <v>0</v>
       </c>
       <c r="S38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T38">
         <v>0</v>
@@ -9044,7 +7742,7 @@
         <v>0</v>
       </c>
       <c r="AP38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ38">
         <v>0</v>
@@ -9068,16 +7766,16 @@
         <v>0</v>
       </c>
       <c r="AX38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY38">
         <v>0</v>
       </c>
       <c r="AZ38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB38">
         <v>3</v>
@@ -9092,22 +7790,22 @@
         <v>3</v>
       </c>
       <c r="BF38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BG38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BH38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BI38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BJ38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BK38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BL38">
         <v>9</v>
@@ -9136,28 +7834,28 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I39">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K39">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L39">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M39">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N39">
         <v>3</v>
       </c>
       <c r="O39">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P39">
         <v>0</v>
@@ -9169,7 +7867,7 @@
         <v>0</v>
       </c>
       <c r="S39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T39">
         <v>0</v>
@@ -9208,7 +7906,7 @@
         <v>0</v>
       </c>
       <c r="AF39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG39">
         <v>0</v>
@@ -9238,7 +7936,7 @@
         <v>0</v>
       </c>
       <c r="AP39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ39">
         <v>0</v>
@@ -9262,19 +7960,19 @@
         <v>0</v>
       </c>
       <c r="AX39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY39">
         <v>0</v>
       </c>
       <c r="AZ39">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA39">
         <v>0</v>
       </c>
       <c r="BB39">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BC39">
         <v>0</v>
@@ -9348,10 +8046,10 @@
         <v>0</v>
       </c>
       <c r="N40">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P40">
         <v>0</v>
@@ -9363,7 +8061,7 @@
         <v>0</v>
       </c>
       <c r="S40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T40">
         <v>0</v>
@@ -9432,7 +8130,7 @@
         <v>0</v>
       </c>
       <c r="AP40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ40">
         <v>0</v>
@@ -9456,19 +8154,19 @@
         <v>0</v>
       </c>
       <c r="AX40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY40">
         <v>0</v>
       </c>
       <c r="AZ40">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA40">
         <v>0</v>
       </c>
       <c r="BB40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BC40">
         <v>0</v>
@@ -9542,10 +8240,10 @@
         <v>0</v>
       </c>
       <c r="N41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O41">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P41">
         <v>0</v>
@@ -9557,7 +8255,7 @@
         <v>0</v>
       </c>
       <c r="S41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T41">
         <v>0</v>
@@ -9626,7 +8324,7 @@
         <v>0</v>
       </c>
       <c r="AP41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ41">
         <v>0</v>
@@ -9650,19 +8348,19 @@
         <v>0</v>
       </c>
       <c r="AX41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY41">
         <v>0</v>
       </c>
       <c r="AZ41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA41">
         <v>0</v>
       </c>
       <c r="BB41">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BC41">
         <v>0</v>
@@ -9736,10 +8434,10 @@
         <v>0</v>
       </c>
       <c r="N42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O42">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P42">
         <v>0</v>
@@ -9751,7 +8449,7 @@
         <v>0</v>
       </c>
       <c r="S42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T42">
         <v>0</v>
@@ -9820,7 +8518,7 @@
         <v>0</v>
       </c>
       <c r="AP42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ42">
         <v>0</v>
@@ -9838,25 +8536,25 @@
         <v>0</v>
       </c>
       <c r="AV42">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AW42">
         <v>0</v>
       </c>
       <c r="AX42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY42">
         <v>0</v>
       </c>
       <c r="AZ42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA42">
         <v>0</v>
       </c>
       <c r="BB42">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BC42">
         <v>0</v>
@@ -9930,10 +8628,10 @@
         <v>0</v>
       </c>
       <c r="N43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O43">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P43">
         <v>0</v>
@@ -9945,7 +8643,7 @@
         <v>0</v>
       </c>
       <c r="S43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T43">
         <v>0</v>
@@ -9954,7 +8652,7 @@
         <v>0</v>
       </c>
       <c r="V43">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W43">
         <v>0</v>
@@ -10014,7 +8712,7 @@
         <v>0</v>
       </c>
       <c r="AP43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ43">
         <v>0</v>
@@ -10038,19 +8736,19 @@
         <v>0</v>
       </c>
       <c r="AX43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY43">
         <v>0</v>
       </c>
       <c r="AZ43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA43">
         <v>0</v>
       </c>
       <c r="BB43">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BC43">
         <v>0</v>
@@ -10124,10 +8822,10 @@
         <v>0</v>
       </c>
       <c r="N44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O44">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P44">
         <v>0</v>
@@ -10139,7 +8837,7 @@
         <v>0</v>
       </c>
       <c r="S44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T44">
         <v>0</v>
@@ -10154,7 +8852,7 @@
         <v>0</v>
       </c>
       <c r="X44">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y44">
         <v>0</v>
@@ -10202,13 +8900,13 @@
         <v>0</v>
       </c>
       <c r="AN44">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AO44">
         <v>0</v>
       </c>
       <c r="AP44">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AQ44">
         <v>0</v>
@@ -10232,19 +8930,19 @@
         <v>0</v>
       </c>
       <c r="AX44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY44">
         <v>0</v>
       </c>
       <c r="AZ44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA44">
         <v>0</v>
       </c>
       <c r="BB44">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BC44">
         <v>0</v>
@@ -10318,10 +9016,10 @@
         <v>0</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O45">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P45">
         <v>0</v>
@@ -10333,7 +9031,7 @@
         <v>0</v>
       </c>
       <c r="S45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T45">
         <v>0</v>
@@ -10402,7 +9100,7 @@
         <v>0</v>
       </c>
       <c r="AP45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ45">
         <v>0</v>
@@ -10426,13 +9124,13 @@
         <v>0</v>
       </c>
       <c r="AX45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY45">
         <v>0</v>
       </c>
       <c r="AZ45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA45">
         <v>0</v>
@@ -10512,7 +9210,7 @@
         <v>0</v>
       </c>
       <c r="N46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -10527,7 +9225,7 @@
         <v>0</v>
       </c>
       <c r="S46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T46">
         <v>0</v>
@@ -10596,7 +9294,7 @@
         <v>0</v>
       </c>
       <c r="AP46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ46">
         <v>0</v>
@@ -10620,13 +9318,13 @@
         <v>0</v>
       </c>
       <c r="AX46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY46">
         <v>0</v>
       </c>
       <c r="AZ46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA46">
         <v>0</v>
@@ -10706,7 +9404,7 @@
         <v>0</v>
       </c>
       <c r="N47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O47">
         <v>0</v>
@@ -10721,7 +9419,7 @@
         <v>0</v>
       </c>
       <c r="S47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T47">
         <v>0</v>
@@ -10790,7 +9488,7 @@
         <v>0</v>
       </c>
       <c r="AP47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ47">
         <v>0</v>
@@ -10814,13 +9512,13 @@
         <v>0</v>
       </c>
       <c r="AX47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY47">
         <v>0</v>
       </c>
       <c r="AZ47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA47">
         <v>0</v>
@@ -11055,59 +9753,35 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AM9">
-    <cfRule type="cellIs" dxfId="137" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR14">
-    <cfRule type="cellIs" dxfId="135" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>